<commit_message>
Commit 5 - events page test 4
</commit_message>
<xml_diff>
--- a/Events.xlsx
+++ b/Events.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>ImageURL</t>
   </si>
@@ -33,27 +33,18 @@
     <t>Summer Festival</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1zfbdyOKOxFrv9YRL7Dim9rcICJz9T_r9/view?usp=drive_link</t>
-  </si>
-  <si>
     <t>A fun-filled summer music festival.</t>
   </si>
   <si>
     <t>Winter Wonderland</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1fW4E0R7UKI1dGFQul4vJwyCjZtI1ooxL/view?usp=drive_link</t>
-  </si>
-  <si>
     <t>Celebrate the holiday season.</t>
   </si>
   <si>
     <t>Spring Blossom</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/14J5gBGPtxJl9FUC638lID27PKfvrk0Uq/view?usp=drive_link</t>
-  </si>
-  <si>
     <t>Experience the beauty of spring flowers.</t>
   </si>
   <si>
@@ -223,6 +214,9 @@
   </si>
   <si>
     <t>A visual treat of colorful flowers.</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/uc?export=view&amp;id=1fW4E0R7UKI1dGFQul4vJwyCjZtI1ooxL</t>
   </si>
 </sst>
 </file>
@@ -582,15 +576,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="116.7109375" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
   </cols>
   <sheetData>
@@ -608,7 +602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -616,465 +610,440 @@
         <v>45636</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>45651</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>45731</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
+      <c r="C4" t="s">
+        <v>66</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <v>45616</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>5</v>
+      <c r="C5" t="s">
+        <v>66</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>45570</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
+      <c r="C6" t="s">
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
         <v>45677</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
+      <c r="C7" t="s">
+        <v>66</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>45700</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
+      <c r="C8" t="s">
+        <v>66</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>45543</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
+      <c r="C9" t="s">
+        <v>66</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>45597</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
+      <c r="C10" t="s">
+        <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2">
         <v>45741</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2">
         <v>45656</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
         <v>45667</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
+      <c r="C13" t="s">
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
         <v>45614</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>5</v>
+      <c r="C14" t="s">
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2">
         <v>45693</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>8</v>
+      <c r="C15" t="s">
+        <v>66</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2">
         <v>45728</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>11</v>
+      <c r="C16" t="s">
+        <v>66</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2">
         <v>45590</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>5</v>
+      <c r="C17" t="s">
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2">
         <v>45641</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
+      <c r="C18" t="s">
+        <v>66</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2">
         <v>45685</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
+      <c r="C19" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2">
         <v>45608</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2">
         <v>45584</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2">
         <v>45565</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>11</v>
+      <c r="C22" t="s">
+        <v>66</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B23" s="2">
         <v>45726</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>5</v>
+      <c r="C23" t="s">
+        <v>66</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2">
         <v>45631</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>8</v>
+      <c r="C24" t="s">
+        <v>66</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25" s="2">
         <v>45672</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>11</v>
+      <c r="C25" t="s">
+        <v>66</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" s="2">
         <v>45623</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
+      <c r="C26" t="s">
+        <v>66</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B27" s="2">
         <v>45644</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>8</v>
+      <c r="C27" t="s">
+        <v>66</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B28" s="2">
         <v>45716</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>11</v>
+      <c r="C28" t="s">
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B29" s="2">
         <v>45736</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
+      <c r="C29" t="s">
+        <v>66</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B30" s="2">
         <v>45580</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>8</v>
+      <c r="C30" t="s">
+        <v>66</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B31" s="2">
         <v>45634</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>11</v>
+      <c r="C31" t="s">
+        <v>66</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2">
         <v>45721</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>11</v>
+      <c r="C32" t="s">
+        <v>66</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C10" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C13" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C16" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C19" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
-    <hyperlink ref="C22" r:id="rId18"/>
-    <hyperlink ref="C20" r:id="rId19"/>
-    <hyperlink ref="C21" r:id="rId20"/>
-    <hyperlink ref="C25" r:id="rId21"/>
-    <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C28" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C29" r:id="rId27"/>
-    <hyperlink ref="C30" r:id="rId28"/>
-    <hyperlink ref="C31" r:id="rId29"/>
-    <hyperlink ref="C32" r:id="rId30"/>
-    <hyperlink ref="C2" r:id="rId31"/>
+    <hyperlink ref="C11" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId4"/>
+    <hyperlink ref="C20" r:id="rId5"/>
+    <hyperlink ref="C21" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>